<commit_message>
Fixed biomethane in EB's file
</commit_message>
<xml_diff>
--- a/data/SJV Portfolio Tool Spreadsheet - EBetancourt-TheExpectedPortfolio EDITED.xlsx
+++ b/data/SJV Portfolio Tool Spreadsheet - EBetancourt-TheExpectedPortfolio EDITED.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nidhi/Library/CloudStorage/OneDrive-RANDCorporation/CATF/SJV-/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650BCDB4-64C0-2749-9832-3A443AC1E397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D08C7B8E-41C6-1145-879E-C89655313069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="880" windowWidth="36000" windowHeight="20800" activeTab="3" xr2:uid="{3EB5D1B8-C67A-D54A-8FBA-1478F31DBAA7}"/>
+    <workbookView xWindow="2120" yWindow="880" windowWidth="36000" windowHeight="20800" activeTab="2" xr2:uid="{3EB5D1B8-C67A-D54A-8FBA-1478F31DBAA7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -610,7 +610,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -642,14 +642,13 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -694,10 +693,10 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1023,7 +1022,7 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1041,16 +1040,16 @@
       <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:6" ht="115" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19" t="s">
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
     </row>
     <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
@@ -1544,399 +1543,399 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="C1" s="22">
+      <c r="C1" s="21">
         <v>2025</v>
       </c>
-      <c r="D1" s="22">
+      <c r="D1" s="21">
         <v>2026</v>
       </c>
-      <c r="E1" s="22">
+      <c r="E1" s="21">
         <v>2027</v>
       </c>
-      <c r="F1" s="22">
+      <c r="F1" s="21">
         <v>2028</v>
       </c>
-      <c r="G1" s="22">
+      <c r="G1" s="21">
         <v>2029</v>
       </c>
-      <c r="H1" s="22">
+      <c r="H1" s="21">
         <v>2030</v>
       </c>
-      <c r="I1" s="22">
+      <c r="I1" s="21">
         <v>2031</v>
       </c>
-      <c r="J1" s="22">
+      <c r="J1" s="21">
         <v>2032</v>
       </c>
-      <c r="K1" s="22">
+      <c r="K1" s="21">
         <v>2033</v>
       </c>
-      <c r="L1" s="22">
+      <c r="L1" s="21">
         <v>2034</v>
       </c>
-      <c r="M1" s="22">
+      <c r="M1" s="21">
         <v>2035</v>
       </c>
-      <c r="N1" s="22">
+      <c r="N1" s="21">
         <v>2036</v>
       </c>
-      <c r="O1" s="22">
+      <c r="O1" s="21">
         <v>2037</v>
       </c>
-      <c r="P1" s="22">
+      <c r="P1" s="21">
         <v>2038</v>
       </c>
-      <c r="Q1" s="22">
+      <c r="Q1" s="21">
         <v>2039</v>
       </c>
-      <c r="R1" s="22">
+      <c r="R1" s="21">
         <v>2040</v>
       </c>
-      <c r="S1" s="22">
+      <c r="S1" s="21">
         <v>2041</v>
       </c>
-      <c r="T1" s="22">
+      <c r="T1" s="21">
         <v>2042</v>
       </c>
-      <c r="U1" s="22">
+      <c r="U1" s="21">
         <v>2043</v>
       </c>
-      <c r="V1" s="22">
+      <c r="V1" s="21">
         <v>2044</v>
       </c>
-      <c r="W1" s="22">
+      <c r="W1" s="21">
         <v>2045</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A2" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="22" t="s">
+      <c r="A2" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="C2" s="22">
-        <v>1</v>
-      </c>
-      <c r="D2" s="22">
-        <v>1</v>
-      </c>
-      <c r="E2" s="22">
-        <v>1</v>
-      </c>
-      <c r="F2" s="22">
-        <v>1</v>
-      </c>
-      <c r="G2" s="22">
-        <v>1</v>
-      </c>
-      <c r="H2" s="22">
-        <v>1</v>
-      </c>
-      <c r="I2" s="22">
-        <v>1</v>
-      </c>
-      <c r="J2" s="22">
-        <v>1</v>
-      </c>
-      <c r="K2" s="22">
-        <v>1</v>
-      </c>
-      <c r="L2" s="22">
-        <v>1</v>
-      </c>
-      <c r="M2" s="22">
-        <v>1</v>
-      </c>
-      <c r="N2" s="22">
-        <v>1</v>
-      </c>
-      <c r="O2" s="22">
-        <v>1</v>
-      </c>
-      <c r="P2" s="22">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="22">
-        <v>1</v>
-      </c>
-      <c r="R2" s="22">
-        <v>1</v>
-      </c>
-      <c r="S2" s="22">
-        <v>1</v>
-      </c>
-      <c r="T2" s="22">
-        <v>1</v>
-      </c>
-      <c r="U2" s="22">
-        <v>1</v>
-      </c>
-      <c r="V2" s="22">
-        <v>1</v>
-      </c>
-      <c r="W2" s="22">
+      <c r="C2" s="21">
+        <v>1</v>
+      </c>
+      <c r="D2" s="21">
+        <v>1</v>
+      </c>
+      <c r="E2" s="21">
+        <v>1</v>
+      </c>
+      <c r="F2" s="21">
+        <v>1</v>
+      </c>
+      <c r="G2" s="21">
+        <v>1</v>
+      </c>
+      <c r="H2" s="21">
+        <v>1</v>
+      </c>
+      <c r="I2" s="21">
+        <v>1</v>
+      </c>
+      <c r="J2" s="21">
+        <v>1</v>
+      </c>
+      <c r="K2" s="21">
+        <v>1</v>
+      </c>
+      <c r="L2" s="21">
+        <v>1</v>
+      </c>
+      <c r="M2" s="21">
+        <v>1</v>
+      </c>
+      <c r="N2" s="21">
+        <v>1</v>
+      </c>
+      <c r="O2" s="21">
+        <v>1</v>
+      </c>
+      <c r="P2" s="21">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="21">
+        <v>1</v>
+      </c>
+      <c r="R2" s="21">
+        <v>1</v>
+      </c>
+      <c r="S2" s="21">
+        <v>1</v>
+      </c>
+      <c r="T2" s="21">
+        <v>1</v>
+      </c>
+      <c r="U2" s="21">
+        <v>1</v>
+      </c>
+      <c r="V2" s="21">
+        <v>1</v>
+      </c>
+      <c r="W2" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="C3" s="23">
+      <c r="C3" s="22">
         <f>Sheet1!B34</f>
         <v>0.8</v>
       </c>
-      <c r="D3" s="23">
+      <c r="D3" s="22">
         <f>Sheet1!C34</f>
         <v>0</v>
       </c>
-      <c r="E3" s="23">
+      <c r="E3" s="22">
         <f>Sheet1!D34</f>
         <v>0</v>
       </c>
-      <c r="F3" s="23">
+      <c r="F3" s="22">
         <f>Sheet1!E34</f>
         <v>0</v>
       </c>
-      <c r="G3" s="23">
+      <c r="G3" s="22">
         <f>Sheet1!F34</f>
         <v>0</v>
       </c>
-      <c r="H3" s="23">
+      <c r="H3" s="22">
         <f>Sheet1!G34</f>
         <v>0</v>
       </c>
-      <c r="I3" s="23">
+      <c r="I3" s="22">
         <f>Sheet1!H34</f>
         <v>0</v>
       </c>
-      <c r="J3" s="23">
+      <c r="J3" s="22">
         <f>Sheet1!I34</f>
         <v>0</v>
       </c>
-      <c r="K3" s="23">
+      <c r="K3" s="22">
         <f>Sheet1!J34</f>
         <v>0</v>
       </c>
-      <c r="L3" s="23">
+      <c r="L3" s="22">
         <f>Sheet1!K34</f>
         <v>0</v>
       </c>
-      <c r="M3" s="23">
+      <c r="M3" s="22">
         <f>Sheet1!L34</f>
         <v>0</v>
       </c>
-      <c r="N3" s="23">
+      <c r="N3" s="22">
         <f>Sheet1!M34</f>
         <v>0</v>
       </c>
-      <c r="O3" s="23">
+      <c r="O3" s="22">
         <f>Sheet1!N34</f>
         <v>0</v>
       </c>
-      <c r="P3" s="23">
+      <c r="P3" s="22">
         <f>Sheet1!O34</f>
         <v>0</v>
       </c>
-      <c r="Q3" s="23">
+      <c r="Q3" s="22">
         <f>Sheet1!P34</f>
         <v>0</v>
       </c>
-      <c r="R3" s="23">
+      <c r="R3" s="22">
         <f>Sheet1!Q34</f>
         <v>0</v>
       </c>
-      <c r="S3" s="23">
+      <c r="S3" s="22">
         <f>Sheet1!R34</f>
         <v>0</v>
       </c>
-      <c r="T3" s="23">
+      <c r="T3" s="22">
         <f>Sheet1!S34</f>
         <v>0</v>
       </c>
-      <c r="U3" s="23">
+      <c r="U3" s="22">
         <f>Sheet1!T34</f>
         <v>0</v>
       </c>
-      <c r="V3" s="23">
+      <c r="V3" s="22">
         <f>Sheet1!U34</f>
         <v>0</v>
       </c>
-      <c r="W3" s="23">
+      <c r="W3" s="22">
         <f>Sheet1!V34</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="C4" s="23">
+      <c r="C4" s="22">
         <f>Sheet1!B35</f>
         <v>0.2</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="22">
         <f>Sheet1!C35</f>
         <v>0</v>
       </c>
-      <c r="E4" s="23">
+      <c r="E4" s="22">
         <f>Sheet1!D35</f>
         <v>0</v>
       </c>
-      <c r="F4" s="23">
+      <c r="F4" s="22">
         <f>Sheet1!E35</f>
         <v>0</v>
       </c>
-      <c r="G4" s="23">
+      <c r="G4" s="22">
         <f>Sheet1!F35</f>
         <v>0</v>
       </c>
-      <c r="H4" s="23">
+      <c r="H4" s="22">
         <f>Sheet1!G35</f>
         <v>0</v>
       </c>
-      <c r="I4" s="23">
+      <c r="I4" s="22">
         <f>Sheet1!H35</f>
         <v>0</v>
       </c>
-      <c r="J4" s="23">
+      <c r="J4" s="22">
         <f>Sheet1!I35</f>
         <v>0</v>
       </c>
-      <c r="K4" s="23">
+      <c r="K4" s="22">
         <f>Sheet1!J35</f>
         <v>0</v>
       </c>
-      <c r="L4" s="23">
+      <c r="L4" s="22">
         <f>Sheet1!K35</f>
         <v>0</v>
       </c>
-      <c r="M4" s="23">
+      <c r="M4" s="22">
         <f>Sheet1!L35</f>
         <v>0</v>
       </c>
-      <c r="N4" s="23">
+      <c r="N4" s="22">
         <f>Sheet1!M35</f>
         <v>0</v>
       </c>
-      <c r="O4" s="23">
+      <c r="O4" s="22">
         <f>Sheet1!N35</f>
         <v>0</v>
       </c>
-      <c r="P4" s="23">
+      <c r="P4" s="22">
         <f>Sheet1!O35</f>
         <v>0</v>
       </c>
-      <c r="Q4" s="23">
+      <c r="Q4" s="22">
         <f>Sheet1!P35</f>
         <v>0</v>
       </c>
-      <c r="R4" s="23">
+      <c r="R4" s="22">
         <f>Sheet1!Q35</f>
         <v>0</v>
       </c>
-      <c r="S4" s="23">
+      <c r="S4" s="22">
         <f>Sheet1!R35</f>
         <v>0</v>
       </c>
-      <c r="T4" s="23">
+      <c r="T4" s="22">
         <f>Sheet1!S35</f>
         <v>0</v>
       </c>
-      <c r="U4" s="23">
+      <c r="U4" s="22">
         <f>Sheet1!T35</f>
         <v>0</v>
       </c>
-      <c r="V4" s="23">
+      <c r="V4" s="22">
         <f>Sheet1!U35</f>
         <v>0</v>
       </c>
-      <c r="W4" s="23">
+      <c r="W4" s="22">
         <f>Sheet1!V35</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="C5" s="22">
-        <v>1</v>
-      </c>
-      <c r="D5" s="22">
-        <v>1</v>
-      </c>
-      <c r="E5" s="22">
-        <v>1</v>
-      </c>
-      <c r="F5" s="22">
-        <v>1</v>
-      </c>
-      <c r="G5" s="22">
-        <v>1</v>
-      </c>
-      <c r="H5" s="22">
-        <v>1</v>
-      </c>
-      <c r="I5" s="22">
-        <v>1</v>
-      </c>
-      <c r="J5" s="22">
-        <v>1</v>
-      </c>
-      <c r="K5" s="22">
-        <v>1</v>
-      </c>
-      <c r="L5" s="22">
-        <v>1</v>
-      </c>
-      <c r="M5" s="22">
-        <v>1</v>
-      </c>
-      <c r="N5" s="22">
-        <v>1</v>
-      </c>
-      <c r="O5" s="22">
-        <v>1</v>
-      </c>
-      <c r="P5" s="22">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="22">
-        <v>1</v>
-      </c>
-      <c r="R5" s="22">
-        <v>1</v>
-      </c>
-      <c r="S5" s="22">
-        <v>1</v>
-      </c>
-      <c r="T5" s="22">
-        <v>1</v>
-      </c>
-      <c r="U5" s="22">
-        <v>1</v>
-      </c>
-      <c r="V5" s="22">
-        <v>1</v>
-      </c>
-      <c r="W5" s="22">
+      <c r="C5" s="21">
+        <v>1</v>
+      </c>
+      <c r="D5" s="21">
+        <v>1</v>
+      </c>
+      <c r="E5" s="21">
+        <v>1</v>
+      </c>
+      <c r="F5" s="21">
+        <v>1</v>
+      </c>
+      <c r="G5" s="21">
+        <v>1</v>
+      </c>
+      <c r="H5" s="21">
+        <v>1</v>
+      </c>
+      <c r="I5" s="21">
+        <v>1</v>
+      </c>
+      <c r="J5" s="21">
+        <v>1</v>
+      </c>
+      <c r="K5" s="21">
+        <v>1</v>
+      </c>
+      <c r="L5" s="21">
+        <v>1</v>
+      </c>
+      <c r="M5" s="21">
+        <v>1</v>
+      </c>
+      <c r="N5" s="21">
+        <v>1</v>
+      </c>
+      <c r="O5" s="21">
+        <v>1</v>
+      </c>
+      <c r="P5" s="21">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="21">
+        <v>1</v>
+      </c>
+      <c r="R5" s="21">
+        <v>1</v>
+      </c>
+      <c r="S5" s="21">
+        <v>1</v>
+      </c>
+      <c r="T5" s="21">
+        <v>1</v>
+      </c>
+      <c r="U5" s="21">
+        <v>1</v>
+      </c>
+      <c r="V5" s="21">
+        <v>1</v>
+      </c>
+      <c r="W5" s="21">
         <v>1</v>
       </c>
     </row>
@@ -2162,8 +2161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AB86C67-1FB8-CB44-BDCD-F09BD6DE6122}">
   <dimension ref="A1:AA18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AA14" sqref="AA14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2276,7 +2275,7 @@
       <c r="F2" t="s">
         <v>76</v>
       </c>
-      <c r="G2" s="21">
+      <c r="G2" s="20">
         <f>AA2/21</f>
         <v>1428.5714285714287</v>
       </c>
@@ -2285,7 +2284,7 @@
         <v>2857.1428571428573</v>
       </c>
       <c r="I2">
-        <f t="shared" ref="I2:X13" si="0">$AA2/21+H2</f>
+        <f t="shared" ref="I2:X2" si="0">$AA2/21+H2</f>
         <v>4285.7142857142862</v>
       </c>
       <c r="J2">
@@ -2380,7 +2379,7 @@
       <c r="F3" t="s">
         <v>76</v>
       </c>
-      <c r="G3" s="21">
+      <c r="G3" s="20">
         <f t="shared" ref="G3:G18" si="2">AA3/21</f>
         <v>0</v>
       </c>
@@ -2484,7 +2483,7 @@
       <c r="F4" t="s">
         <v>76</v>
       </c>
-      <c r="G4" s="21">
+      <c r="G4" s="20">
         <f t="shared" si="2"/>
         <v>761.90476190476193</v>
       </c>
@@ -2588,7 +2587,7 @@
       <c r="F5" t="s">
         <v>76</v>
       </c>
-      <c r="G5" s="21">
+      <c r="G5" s="20">
         <f t="shared" si="2"/>
         <v>47.61904761904762</v>
       </c>
@@ -2692,7 +2691,7 @@
       <c r="F6" t="s">
         <v>76</v>
       </c>
-      <c r="G6" s="21">
+      <c r="G6" s="20">
         <f t="shared" si="2"/>
         <v>4.7619047619047619</v>
       </c>
@@ -2796,7 +2795,7 @@
       <c r="F7" t="s">
         <v>76</v>
       </c>
-      <c r="G7" s="21">
+      <c r="G7" s="20">
         <f t="shared" si="2"/>
         <v>2.3809523809523809</v>
       </c>
@@ -2900,7 +2899,7 @@
       <c r="F8" t="s">
         <v>76</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G8" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3004,7 +3003,7 @@
       <c r="F9" t="s">
         <v>85</v>
       </c>
-      <c r="G9" s="21">
+      <c r="G9" s="20">
         <f t="shared" si="2"/>
         <v>14285.714285714286</v>
       </c>
@@ -3084,7 +3083,7 @@
         <f t="shared" si="1"/>
         <v>285714.28571428574</v>
       </c>
-      <c r="AA9" s="21">
+      <c r="AA9" s="20">
         <f>Sheet1!C12*1000</f>
         <v>300000</v>
       </c>
@@ -3108,7 +3107,7 @@
       <c r="F10" t="s">
         <v>85</v>
       </c>
-      <c r="G10" s="21">
+      <c r="G10" s="20">
         <f t="shared" si="2"/>
         <v>523.80952380952385</v>
       </c>
@@ -3188,7 +3187,7 @@
         <f t="shared" si="1"/>
         <v>10476.190476190473</v>
       </c>
-      <c r="AA10" s="21">
+      <c r="AA10" s="20">
         <f>Sheet1!C13*1000</f>
         <v>11000</v>
       </c>
@@ -3212,7 +3211,7 @@
       <c r="F11" t="s">
         <v>85</v>
       </c>
-      <c r="G11" s="21">
+      <c r="G11" s="20">
         <f t="shared" si="2"/>
         <v>19047.619047619046</v>
       </c>
@@ -3292,7 +3291,7 @@
         <f t="shared" si="1"/>
         <v>380952.38095238101</v>
       </c>
-      <c r="AA11" s="21">
+      <c r="AA11" s="20">
         <f>Sheet1!C14*1000</f>
         <v>400000</v>
       </c>
@@ -3316,7 +3315,7 @@
       <c r="F12" t="s">
         <v>85</v>
       </c>
-      <c r="G12" s="21">
+      <c r="G12" s="20">
         <f t="shared" si="2"/>
         <v>14285.714285714286</v>
       </c>
@@ -3396,7 +3395,7 @@
         <f t="shared" si="1"/>
         <v>285714.28571428574</v>
       </c>
-      <c r="AA12" s="21">
+      <c r="AA12" s="20">
         <f>Sheet1!C15*1000</f>
         <v>300000</v>
       </c>
@@ -3420,89 +3419,88 @@
       <c r="F13" t="s">
         <v>85</v>
       </c>
-      <c r="G13" s="21">
-        <f t="shared" si="2"/>
+      <c r="G13" s="20">
+        <f>AA13/21</f>
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <f>$AA14/21+G13</f>
         <v>142.85714285714286</v>
       </c>
-      <c r="H13">
-        <f t="shared" si="3"/>
+      <c r="I13">
+        <f>$AA14/21+H13</f>
         <v>285.71428571428572</v>
       </c>
-      <c r="I13">
-        <f t="shared" si="3"/>
+      <c r="J13">
+        <f>$AA14/21+I13</f>
         <v>428.57142857142856</v>
       </c>
-      <c r="J13">
-        <f t="shared" si="3"/>
+      <c r="K13">
+        <f>$AA14/21+J13</f>
         <v>571.42857142857144</v>
       </c>
-      <c r="K13">
-        <f t="shared" si="3"/>
+      <c r="L13">
+        <f>$AA14/21+K13</f>
         <v>714.28571428571433</v>
       </c>
-      <c r="L13">
-        <f t="shared" si="3"/>
+      <c r="M13">
+        <f>$AA14/21+L13</f>
         <v>857.14285714285722</v>
       </c>
-      <c r="M13">
-        <f t="shared" si="3"/>
+      <c r="N13">
+        <f>$AA14/21+M13</f>
         <v>1000.0000000000001</v>
       </c>
-      <c r="N13">
-        <f t="shared" si="3"/>
+      <c r="O13">
+        <f>$AA14/21+N13</f>
         <v>1142.8571428571429</v>
       </c>
-      <c r="O13">
-        <f t="shared" si="3"/>
+      <c r="P13">
+        <f>$AA14/21+O13</f>
         <v>1285.7142857142858</v>
       </c>
-      <c r="P13">
-        <f t="shared" si="3"/>
+      <c r="Q13">
+        <f>$AA14/21+P13</f>
         <v>1428.5714285714287</v>
       </c>
-      <c r="Q13">
-        <f t="shared" si="3"/>
+      <c r="R13">
+        <f>$AA14/21+Q13</f>
         <v>1571.4285714285716</v>
       </c>
-      <c r="R13">
-        <f t="shared" si="3"/>
+      <c r="S13">
+        <f>$AA14/21+R13</f>
         <v>1714.2857142857144</v>
       </c>
-      <c r="S13">
-        <f t="shared" si="3"/>
+      <c r="T13">
+        <f>$AA14/21+S13</f>
         <v>1857.1428571428573</v>
       </c>
-      <c r="T13">
-        <f t="shared" si="3"/>
+      <c r="U13">
+        <f>$AA14/21+T13</f>
         <v>2000.0000000000002</v>
       </c>
-      <c r="U13">
-        <f t="shared" si="3"/>
+      <c r="V13">
+        <f>$AA14/21+U13</f>
         <v>2142.8571428571431</v>
       </c>
-      <c r="V13">
-        <f t="shared" si="3"/>
+      <c r="W13">
+        <f>$AA14/21+V13</f>
         <v>2285.7142857142858</v>
       </c>
-      <c r="W13">
-        <f t="shared" si="3"/>
+      <c r="X13">
+        <f>$AA14/21+W13</f>
         <v>2428.5714285714284</v>
       </c>
-      <c r="X13">
-        <f t="shared" si="1"/>
+      <c r="Y13">
+        <f>$AA14/21+X13</f>
         <v>2571.4285714285711</v>
       </c>
-      <c r="Y13">
-        <f t="shared" si="1"/>
+      <c r="Z13">
+        <f>$AA14/21+Y13</f>
         <v>2714.2857142857138</v>
       </c>
-      <c r="Z13">
-        <f t="shared" si="1"/>
-        <v>2857.1428571428564</v>
-      </c>
-      <c r="AA13" s="21">
-        <f>Sheet1!C16*1000</f>
-        <v>3000</v>
+      <c r="AA13">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.2">
@@ -3524,89 +3522,89 @@
       <c r="F14" t="s">
         <v>91</v>
       </c>
-      <c r="G14" s="21">
-        <f t="shared" si="2"/>
-        <v>285.71428571428572</v>
+      <c r="G14" s="20">
+        <f>AA14/21</f>
+        <v>142.85714285714286</v>
       </c>
       <c r="H14">
-        <f t="shared" si="3"/>
-        <v>571.42857142857144</v>
+        <f>$AA15/21+G14</f>
+        <v>428.57142857142856</v>
       </c>
       <c r="I14">
-        <f t="shared" si="3"/>
-        <v>857.14285714285711</v>
+        <f>$AA15/21+H14</f>
+        <v>714.28571428571422</v>
       </c>
       <c r="J14">
-        <f t="shared" si="3"/>
-        <v>1142.8571428571429</v>
+        <f>$AA15/21+I14</f>
+        <v>1000</v>
       </c>
       <c r="K14">
-        <f t="shared" si="3"/>
-        <v>1428.5714285714287</v>
+        <f>$AA15/21+J14</f>
+        <v>1285.7142857142858</v>
       </c>
       <c r="L14">
-        <f t="shared" si="3"/>
-        <v>1714.2857142857144</v>
+        <f>$AA15/21+K14</f>
+        <v>1571.4285714285716</v>
       </c>
       <c r="M14">
-        <f t="shared" si="3"/>
-        <v>2000.0000000000002</v>
+        <f>$AA15/21+L14</f>
+        <v>1857.1428571428573</v>
       </c>
       <c r="N14">
-        <f t="shared" si="3"/>
-        <v>2285.7142857142858</v>
+        <f>$AA15/21+M14</f>
+        <v>2142.8571428571431</v>
       </c>
       <c r="O14">
-        <f t="shared" si="3"/>
-        <v>2571.4285714285716</v>
+        <f>$AA15/21+N14</f>
+        <v>2428.5714285714289</v>
       </c>
       <c r="P14">
-        <f t="shared" si="3"/>
-        <v>2857.1428571428573</v>
+        <f>$AA15/21+O14</f>
+        <v>2714.2857142857147</v>
       </c>
       <c r="Q14">
-        <f t="shared" si="3"/>
-        <v>3142.8571428571431</v>
+        <f>$AA15/21+P14</f>
+        <v>3000.0000000000005</v>
       </c>
       <c r="R14">
-        <f t="shared" si="3"/>
-        <v>3428.5714285714289</v>
+        <f>$AA15/21+Q14</f>
+        <v>3285.7142857142862</v>
       </c>
       <c r="S14">
-        <f t="shared" si="3"/>
-        <v>3714.2857142857147</v>
+        <f>$AA15/21+R14</f>
+        <v>3571.428571428572</v>
       </c>
       <c r="T14">
-        <f t="shared" si="3"/>
-        <v>4000.0000000000005</v>
+        <f>$AA15/21+S14</f>
+        <v>3857.1428571428578</v>
       </c>
       <c r="U14">
-        <f t="shared" si="3"/>
-        <v>4285.7142857142862</v>
+        <f>$AA15/21+T14</f>
+        <v>4142.8571428571431</v>
       </c>
       <c r="V14">
-        <f t="shared" si="3"/>
-        <v>4571.4285714285716</v>
+        <f>$AA15/21+U14</f>
+        <v>4428.5714285714284</v>
       </c>
       <c r="W14">
-        <f t="shared" si="3"/>
-        <v>4857.1428571428569</v>
+        <f>$AA15/21+V14</f>
+        <v>4714.2857142857138</v>
       </c>
       <c r="X14">
-        <f t="shared" si="1"/>
-        <v>5142.8571428571422</v>
+        <f>$AA15/21+W14</f>
+        <v>4999.9999999999991</v>
       </c>
       <c r="Y14">
-        <f t="shared" si="1"/>
-        <v>5428.5714285714275</v>
+        <f>$AA15/21+X14</f>
+        <v>5285.7142857142844</v>
       </c>
       <c r="Z14">
-        <f t="shared" si="1"/>
-        <v>5714.2857142857129</v>
-      </c>
-      <c r="AA14" s="21">
-        <f>Sheet1!C17*1000</f>
-        <v>6000</v>
+        <f>$AA15/21+Y14</f>
+        <v>5571.4285714285697</v>
+      </c>
+      <c r="AA14" s="20">
+        <f>Sheet1!C16*1000</f>
+        <v>3000</v>
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.2">
@@ -3628,89 +3626,89 @@
       <c r="F15" t="s">
         <v>91</v>
       </c>
-      <c r="G15" s="21">
-        <f t="shared" si="2"/>
-        <v>0</v>
+      <c r="G15" s="20">
+        <f>AA15/21</f>
+        <v>285.71428571428572</v>
       </c>
       <c r="H15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>$AA16/21+G15</f>
+        <v>285.71428571428572</v>
       </c>
       <c r="I15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" ref="I15:Z15" si="4">$AA16/21+H15</f>
+        <v>285.71428571428572</v>
       </c>
       <c r="J15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>285.71428571428572</v>
       </c>
       <c r="K15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>285.71428571428572</v>
       </c>
       <c r="L15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>285.71428571428572</v>
       </c>
       <c r="M15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>285.71428571428572</v>
       </c>
       <c r="N15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>285.71428571428572</v>
       </c>
       <c r="O15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>285.71428571428572</v>
       </c>
       <c r="P15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>285.71428571428572</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>285.71428571428572</v>
       </c>
       <c r="R15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>285.71428571428572</v>
       </c>
       <c r="S15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>285.71428571428572</v>
       </c>
       <c r="T15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>285.71428571428572</v>
       </c>
       <c r="U15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>285.71428571428572</v>
       </c>
       <c r="V15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>285.71428571428572</v>
       </c>
       <c r="W15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>285.71428571428572</v>
       </c>
       <c r="X15">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>285.71428571428572</v>
       </c>
       <c r="Y15">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>285.71428571428572</v>
       </c>
       <c r="Z15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AA15" s="21">
-        <f>Sheet1!C18*1000</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>285.71428571428572</v>
+      </c>
+      <c r="AA15" s="20">
+        <f>Sheet1!C17*1000</f>
+        <v>6000</v>
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.2">
@@ -3732,7 +3730,7 @@
       <c r="F16" t="s">
         <v>93</v>
       </c>
-      <c r="G16" s="21">
+      <c r="G16" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3812,7 +3810,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AA16" s="21">
+      <c r="AA16" s="20">
         <f>Sheet1!C19*1000</f>
         <v>0</v>
       </c>
@@ -3836,7 +3834,7 @@
       <c r="F17" t="s">
         <v>93</v>
       </c>
-      <c r="G17" s="21">
+      <c r="G17" s="20">
         <f t="shared" si="2"/>
         <v>119.04761904761905</v>
       </c>
@@ -3916,7 +3914,7 @@
         <f t="shared" si="1"/>
         <v>2380.9523809523816</v>
       </c>
-      <c r="AA17" s="21">
+      <c r="AA17" s="20">
         <f>Sheet1!C20*1000</f>
         <v>2500</v>
       </c>
@@ -3940,7 +3938,7 @@
       <c r="F18" t="s">
         <v>93</v>
       </c>
-      <c r="G18" s="21">
+      <c r="G18" s="20">
         <f t="shared" si="2"/>
         <v>119.04761904761905</v>
       </c>
@@ -4005,22 +4003,22 @@
         <v>1904.7619047619048</v>
       </c>
       <c r="W18">
-        <f t="shared" ref="W18:Z18" si="4">$AA18/21+V18</f>
+        <f t="shared" ref="W18:Z18" si="5">$AA18/21+V18</f>
         <v>2023.8095238095239</v>
       </c>
       <c r="X18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2142.8571428571431</v>
       </c>
       <c r="Y18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2261.9047619047624</v>
       </c>
       <c r="Z18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2380.9523809523816</v>
       </c>
-      <c r="AA18" s="21">
+      <c r="AA18" s="20">
         <f>Sheet1!C21*1000</f>
         <v>2500</v>
       </c>
@@ -4034,8 +4032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{487D7336-B959-4943-BB91-2BE20F62B1C9}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4068,7 +4066,7 @@
       <c r="A4" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="20">
+      <c r="B4" s="19">
         <v>45322</v>
       </c>
     </row>
@@ -4076,7 +4074,7 @@
       <c r="A5" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" t="s">
         <v>101</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed biomethane in EB's Expected Porfolio
</commit_message>
<xml_diff>
--- a/data/SJV Portfolio Tool Spreadsheet - EBetancourt-TheExpectedPortfolio EDITED.xlsx
+++ b/data/SJV Portfolio Tool Spreadsheet - EBetancourt-TheExpectedPortfolio EDITED.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nidhi/Library/CloudStorage/OneDrive-RANDCorporation/CATF/SJV-/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BCF941D-DA92-C047-80C5-00284DDA5C0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A981A2C2-2927-DB4E-B9D6-F3E5639D7BFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20800" activeTab="2" xr2:uid="{3EB5D1B8-C67A-D54A-8FBA-1478F31DBAA7}"/>
   </bookViews>
@@ -18,9 +18,6 @@
     <sheet name="feedstock_to_commodity" sheetId="4" r:id="rId3"/>
     <sheet name="portfolio_metadata" sheetId="3" r:id="rId4"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId5"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -42,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="96">
   <si>
     <t>Solar</t>
   </si>
@@ -380,9 +377,6 @@
   </si>
   <si>
     <t>Gasification + Gas Engine</t>
-  </si>
-  <si>
-    <t>Anaerobic Digestion + Conditioning + Gas Engine</t>
   </si>
   <si>
     <t>PV + Electrolysis</t>
@@ -655,36 +649,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="portfolio_input"/>
-      <sheetName val="portfolio_metadata"/>
-      <sheetName val="feedstock_to_commodity"/>
-      <sheetName val="commodity_to_use"/>
-      <sheetName val="Sheet2"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="14">
-          <cell r="C14">
-            <v>1.4906832298136647E-2</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1007,7 +971,7 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16:C17"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1532,7 +1496,7 @@
         <v>69</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C1" s="21">
         <v>2025</v>
@@ -1603,7 +1567,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C2" s="21">
         <v>1</v>
@@ -1674,7 +1638,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C3" s="22">
         <f>Sheet1!B34</f>
@@ -1766,7 +1730,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C4" s="22">
         <f>Sheet1!B35</f>
@@ -1858,7 +1822,7 @@
         <v>15</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C5" s="21">
         <v>1</v>
@@ -2144,10 +2108,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AB86C67-1FB8-CB44-BDCD-F09BD6DE6122}">
-  <dimension ref="A1:Z18"/>
+  <dimension ref="A1:Z17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2327,7 +2291,7 @@
         <v>25714.285714285714</v>
       </c>
       <c r="X2">
-        <f t="shared" ref="W2:Y17" si="1">$Z2/21+W2</f>
+        <f t="shared" ref="W2:Y16" si="1">$Z2/21+W2</f>
         <v>27142.857142857141</v>
       </c>
       <c r="Y2">
@@ -2356,11 +2320,11 @@
         <v>74</v>
       </c>
       <c r="F3" s="20">
-        <f t="shared" ref="F3:F18" si="2">Z3/21</f>
+        <f t="shared" ref="F3:F17" si="2">Z3/21</f>
         <v>0</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:V18" si="3">$Z3/21+F3</f>
+        <f t="shared" ref="G3:V17" si="3">$Z3/21+F3</f>
         <v>0</v>
       </c>
       <c r="H3">
@@ -2846,111 +2810,111 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B8" t="s">
         <v>79</v>
       </c>
       <c r="C8" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>73</v>
+        <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="F8" s="20">
         <f t="shared" si="2"/>
-        <v>0.7098491570541261</v>
+        <v>14285.714285714286</v>
       </c>
       <c r="G8">
         <f t="shared" si="3"/>
-        <v>1.4196983141082522</v>
+        <v>28571.428571428572</v>
       </c>
       <c r="H8">
         <f t="shared" si="3"/>
-        <v>2.1295474711623781</v>
+        <v>42857.142857142855</v>
       </c>
       <c r="I8">
         <f t="shared" si="3"/>
-        <v>2.8393966282165044</v>
+        <v>57142.857142857145</v>
       </c>
       <c r="J8">
         <f t="shared" si="3"/>
-        <v>3.5492457852706307</v>
+        <v>71428.571428571435</v>
       </c>
       <c r="K8">
         <f t="shared" si="3"/>
-        <v>4.259094942324757</v>
+        <v>85714.285714285725</v>
       </c>
       <c r="L8">
         <f t="shared" si="3"/>
-        <v>4.9689440993788834</v>
+        <v>100000.00000000001</v>
       </c>
       <c r="M8">
         <f t="shared" si="3"/>
-        <v>5.6787932564330097</v>
+        <v>114285.7142857143</v>
       </c>
       <c r="N8">
         <f t="shared" si="3"/>
-        <v>6.388642413487136</v>
+        <v>128571.42857142859</v>
       </c>
       <c r="O8">
         <f t="shared" si="3"/>
-        <v>7.0984915705412623</v>
+        <v>142857.14285714287</v>
       </c>
       <c r="P8">
         <f t="shared" si="3"/>
-        <v>7.8083407275953887</v>
+        <v>157142.85714285716</v>
       </c>
       <c r="Q8">
         <f t="shared" si="3"/>
-        <v>8.5181898846495141</v>
+        <v>171428.57142857145</v>
       </c>
       <c r="R8">
         <f t="shared" si="3"/>
-        <v>9.2280390417036404</v>
+        <v>185714.28571428574</v>
       </c>
       <c r="S8">
         <f t="shared" si="3"/>
-        <v>9.9378881987577667</v>
+        <v>200000.00000000003</v>
       </c>
       <c r="T8">
         <f t="shared" si="3"/>
-        <v>10.647737355811893</v>
+        <v>214285.71428571432</v>
       </c>
       <c r="U8">
         <f t="shared" si="3"/>
-        <v>11.357586512866019</v>
+        <v>228571.42857142861</v>
       </c>
       <c r="V8">
         <f t="shared" si="3"/>
-        <v>12.067435669920146</v>
+        <v>242857.1428571429</v>
       </c>
       <c r="W8">
         <f t="shared" si="1"/>
-        <v>12.777284826974272</v>
+        <v>257142.85714285719</v>
       </c>
       <c r="X8">
         <f t="shared" si="1"/>
-        <v>13.487133984028398</v>
+        <v>271428.57142857148</v>
       </c>
       <c r="Y8">
         <f t="shared" si="1"/>
-        <v>14.196983141082525</v>
-      </c>
-      <c r="Z8">
-        <f>[1]portfolio_input!C14*1000</f>
-        <v>14.906832298136647</v>
+        <v>285714.28571428574</v>
+      </c>
+      <c r="Z8" s="20">
+        <f>Sheet1!C12*1000</f>
+        <v>300000</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -2959,96 +2923,96 @@
         <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F9" s="20">
         <f t="shared" si="2"/>
-        <v>14285.714285714286</v>
+        <v>523.80952380952385</v>
       </c>
       <c r="G9">
         <f t="shared" si="3"/>
-        <v>28571.428571428572</v>
+        <v>1047.6190476190477</v>
       </c>
       <c r="H9">
         <f t="shared" si="3"/>
-        <v>42857.142857142855</v>
+        <v>1571.4285714285716</v>
       </c>
       <c r="I9">
         <f t="shared" si="3"/>
-        <v>57142.857142857145</v>
+        <v>2095.2380952380954</v>
       </c>
       <c r="J9">
         <f t="shared" si="3"/>
-        <v>71428.571428571435</v>
+        <v>2619.0476190476193</v>
       </c>
       <c r="K9">
         <f t="shared" si="3"/>
-        <v>85714.285714285725</v>
+        <v>3142.8571428571431</v>
       </c>
       <c r="L9">
         <f t="shared" si="3"/>
-        <v>100000.00000000001</v>
+        <v>3666.666666666667</v>
       </c>
       <c r="M9">
         <f t="shared" si="3"/>
-        <v>114285.7142857143</v>
+        <v>4190.4761904761908</v>
       </c>
       <c r="N9">
         <f t="shared" si="3"/>
-        <v>128571.42857142859</v>
+        <v>4714.2857142857147</v>
       </c>
       <c r="O9">
         <f t="shared" si="3"/>
-        <v>142857.14285714287</v>
+        <v>5238.0952380952385</v>
       </c>
       <c r="P9">
         <f t="shared" si="3"/>
-        <v>157142.85714285716</v>
+        <v>5761.9047619047624</v>
       </c>
       <c r="Q9">
         <f t="shared" si="3"/>
-        <v>171428.57142857145</v>
+        <v>6285.7142857142862</v>
       </c>
       <c r="R9">
         <f t="shared" si="3"/>
-        <v>185714.28571428574</v>
+        <v>6809.5238095238101</v>
       </c>
       <c r="S9">
         <f t="shared" si="3"/>
-        <v>200000.00000000003</v>
+        <v>7333.3333333333339</v>
       </c>
       <c r="T9">
         <f t="shared" si="3"/>
-        <v>214285.71428571432</v>
+        <v>7857.1428571428578</v>
       </c>
       <c r="U9">
         <f t="shared" si="3"/>
-        <v>228571.42857142861</v>
+        <v>8380.9523809523816</v>
       </c>
       <c r="V9">
         <f t="shared" si="3"/>
-        <v>242857.1428571429</v>
+        <v>8904.7619047619046</v>
       </c>
       <c r="W9">
         <f t="shared" si="1"/>
-        <v>257142.85714285719</v>
+        <v>9428.5714285714275</v>
       </c>
       <c r="X9">
         <f t="shared" si="1"/>
-        <v>271428.57142857148</v>
+        <v>9952.3809523809505</v>
       </c>
       <c r="Y9">
         <f t="shared" si="1"/>
-        <v>285714.28571428574</v>
+        <v>10476.190476190473</v>
       </c>
       <c r="Z9" s="20">
-        <f>Sheet1!C12*1000</f>
-        <v>300000</v>
+        <f>Sheet1!C13*1000</f>
+        <v>11000</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
         <v>82</v>
@@ -3060,99 +3024,99 @@
         <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F10" s="20">
         <f t="shared" si="2"/>
-        <v>523.80952380952385</v>
+        <v>19047.619047619046</v>
       </c>
       <c r="G10">
         <f t="shared" si="3"/>
-        <v>1047.6190476190477</v>
+        <v>38095.238095238092</v>
       </c>
       <c r="H10">
         <f t="shared" si="3"/>
-        <v>1571.4285714285716</v>
+        <v>57142.857142857138</v>
       </c>
       <c r="I10">
         <f t="shared" si="3"/>
-        <v>2095.2380952380954</v>
+        <v>76190.476190476184</v>
       </c>
       <c r="J10">
         <f t="shared" si="3"/>
-        <v>2619.0476190476193</v>
+        <v>95238.095238095237</v>
       </c>
       <c r="K10">
         <f t="shared" si="3"/>
-        <v>3142.8571428571431</v>
+        <v>114285.71428571429</v>
       </c>
       <c r="L10">
         <f t="shared" si="3"/>
-        <v>3666.666666666667</v>
+        <v>133333.33333333334</v>
       </c>
       <c r="M10">
         <f t="shared" si="3"/>
-        <v>4190.4761904761908</v>
+        <v>152380.9523809524</v>
       </c>
       <c r="N10">
         <f t="shared" si="3"/>
-        <v>4714.2857142857147</v>
+        <v>171428.57142857145</v>
       </c>
       <c r="O10">
         <f t="shared" si="3"/>
-        <v>5238.0952380952385</v>
+        <v>190476.1904761905</v>
       </c>
       <c r="P10">
         <f t="shared" si="3"/>
-        <v>5761.9047619047624</v>
+        <v>209523.80952380956</v>
       </c>
       <c r="Q10">
         <f t="shared" si="3"/>
-        <v>6285.7142857142862</v>
+        <v>228571.42857142861</v>
       </c>
       <c r="R10">
         <f t="shared" si="3"/>
-        <v>6809.5238095238101</v>
+        <v>247619.04761904766</v>
       </c>
       <c r="S10">
         <f t="shared" si="3"/>
-        <v>7333.3333333333339</v>
+        <v>266666.66666666669</v>
       </c>
       <c r="T10">
         <f t="shared" si="3"/>
-        <v>7857.1428571428578</v>
+        <v>285714.28571428574</v>
       </c>
       <c r="U10">
         <f t="shared" si="3"/>
-        <v>8380.9523809523816</v>
+        <v>304761.90476190479</v>
       </c>
       <c r="V10">
         <f t="shared" si="3"/>
-        <v>8904.7619047619046</v>
+        <v>323809.52380952385</v>
       </c>
       <c r="W10">
         <f t="shared" si="1"/>
-        <v>9428.5714285714275</v>
+        <v>342857.1428571429</v>
       </c>
       <c r="X10">
         <f t="shared" si="1"/>
-        <v>9952.3809523809505</v>
+        <v>361904.76190476195</v>
       </c>
       <c r="Y10">
         <f t="shared" si="1"/>
-        <v>10476.190476190473</v>
+        <v>380952.38095238101</v>
       </c>
       <c r="Z10" s="20">
-        <f>Sheet1!C13*1000</f>
-        <v>11000</v>
+        <f>Sheet1!C14*1000</f>
+        <v>400000</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
@@ -3161,96 +3125,96 @@
         <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F11" s="20">
         <f t="shared" si="2"/>
-        <v>19047.619047619046</v>
+        <v>14285.714285714286</v>
       </c>
       <c r="G11">
         <f t="shared" si="3"/>
-        <v>38095.238095238092</v>
+        <v>28571.428571428572</v>
       </c>
       <c r="H11">
         <f t="shared" si="3"/>
-        <v>57142.857142857138</v>
+        <v>42857.142857142855</v>
       </c>
       <c r="I11">
         <f t="shared" si="3"/>
-        <v>76190.476190476184</v>
+        <v>57142.857142857145</v>
       </c>
       <c r="J11">
         <f t="shared" si="3"/>
-        <v>95238.095238095237</v>
+        <v>71428.571428571435</v>
       </c>
       <c r="K11">
         <f t="shared" si="3"/>
-        <v>114285.71428571429</v>
+        <v>85714.285714285725</v>
       </c>
       <c r="L11">
         <f t="shared" si="3"/>
-        <v>133333.33333333334</v>
+        <v>100000.00000000001</v>
       </c>
       <c r="M11">
         <f t="shared" si="3"/>
-        <v>152380.9523809524</v>
+        <v>114285.7142857143</v>
       </c>
       <c r="N11">
         <f t="shared" si="3"/>
+        <v>128571.42857142859</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="3"/>
+        <v>142857.14285714287</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="3"/>
+        <v>157142.85714285716</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="3"/>
         <v>171428.57142857145</v>
       </c>
-      <c r="O11">
-        <f t="shared" si="3"/>
-        <v>190476.1904761905</v>
-      </c>
-      <c r="P11">
-        <f t="shared" si="3"/>
-        <v>209523.80952380956</v>
-      </c>
-      <c r="Q11">
+      <c r="R11">
+        <f t="shared" si="3"/>
+        <v>185714.28571428574</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="3"/>
+        <v>200000.00000000003</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="3"/>
+        <v>214285.71428571432</v>
+      </c>
+      <c r="U11">
         <f t="shared" si="3"/>
         <v>228571.42857142861</v>
       </c>
-      <c r="R11">
-        <f t="shared" si="3"/>
-        <v>247619.04761904766</v>
-      </c>
-      <c r="S11">
-        <f t="shared" si="3"/>
-        <v>266666.66666666669</v>
-      </c>
-      <c r="T11">
-        <f t="shared" si="3"/>
-        <v>285714.28571428574</v>
-      </c>
-      <c r="U11">
-        <f t="shared" si="3"/>
-        <v>304761.90476190479</v>
-      </c>
       <c r="V11">
         <f t="shared" si="3"/>
-        <v>323809.52380952385</v>
+        <v>242857.1428571429</v>
       </c>
       <c r="W11">
         <f t="shared" si="1"/>
-        <v>342857.1428571429</v>
+        <v>257142.85714285719</v>
       </c>
       <c r="X11">
         <f t="shared" si="1"/>
-        <v>361904.76190476195</v>
+        <v>271428.57142857148</v>
       </c>
       <c r="Y11">
         <f t="shared" si="1"/>
-        <v>380952.38095238101</v>
+        <v>285714.28571428574</v>
       </c>
       <c r="Z11" s="20">
-        <f>Sheet1!C14*1000</f>
-        <v>400000</v>
+        <f>Sheet1!C15*1000</f>
+        <v>300000</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
         <v>83</v>
@@ -3262,199 +3226,199 @@
         <v>9</v>
       </c>
       <c r="E12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F12" s="20">
-        <f t="shared" si="2"/>
-        <v>14285.714285714286</v>
+        <f>Z12/21</f>
+        <v>0</v>
       </c>
       <c r="G12">
         <f t="shared" si="3"/>
-        <v>28571.428571428572</v>
+        <v>0</v>
       </c>
       <c r="H12">
-        <f t="shared" si="3"/>
-        <v>42857.142857142855</v>
+        <f t="shared" ref="H12" si="4">$Z12/21+G12</f>
+        <v>0</v>
       </c>
       <c r="I12">
-        <f t="shared" si="3"/>
-        <v>57142.857142857145</v>
+        <f t="shared" ref="I12" si="5">$Z12/21+H12</f>
+        <v>0</v>
       </c>
       <c r="J12">
-        <f t="shared" si="3"/>
-        <v>71428.571428571435</v>
+        <f t="shared" ref="J12" si="6">$Z12/21+I12</f>
+        <v>0</v>
       </c>
       <c r="K12">
-        <f t="shared" si="3"/>
-        <v>85714.285714285725</v>
+        <f t="shared" ref="K12" si="7">$Z12/21+J12</f>
+        <v>0</v>
       </c>
       <c r="L12">
-        <f t="shared" si="3"/>
-        <v>100000.00000000001</v>
+        <f t="shared" ref="L12" si="8">$Z12/21+K12</f>
+        <v>0</v>
       </c>
       <c r="M12">
-        <f t="shared" si="3"/>
-        <v>114285.7142857143</v>
+        <f t="shared" ref="M12" si="9">$Z12/21+L12</f>
+        <v>0</v>
       </c>
       <c r="N12">
-        <f t="shared" si="3"/>
-        <v>128571.42857142859</v>
+        <f t="shared" ref="N12" si="10">$Z12/21+M12</f>
+        <v>0</v>
       </c>
       <c r="O12">
-        <f t="shared" si="3"/>
-        <v>142857.14285714287</v>
+        <f t="shared" ref="O12" si="11">$Z12/21+N12</f>
+        <v>0</v>
       </c>
       <c r="P12">
-        <f t="shared" si="3"/>
-        <v>157142.85714285716</v>
+        <f t="shared" ref="P12" si="12">$Z12/21+O12</f>
+        <v>0</v>
       </c>
       <c r="Q12">
-        <f t="shared" si="3"/>
-        <v>171428.57142857145</v>
+        <f t="shared" ref="Q12" si="13">$Z12/21+P12</f>
+        <v>0</v>
       </c>
       <c r="R12">
-        <f t="shared" si="3"/>
-        <v>185714.28571428574</v>
+        <f t="shared" ref="R12" si="14">$Z12/21+Q12</f>
+        <v>0</v>
       </c>
       <c r="S12">
-        <f t="shared" si="3"/>
-        <v>200000.00000000003</v>
+        <f t="shared" ref="S12" si="15">$Z12/21+R12</f>
+        <v>0</v>
       </c>
       <c r="T12">
-        <f t="shared" si="3"/>
-        <v>214285.71428571432</v>
+        <f t="shared" ref="T12" si="16">$Z12/21+S12</f>
+        <v>0</v>
       </c>
       <c r="U12">
-        <f t="shared" si="3"/>
-        <v>228571.42857142861</v>
+        <f t="shared" ref="U12" si="17">$Z12/21+T12</f>
+        <v>0</v>
       </c>
       <c r="V12">
-        <f t="shared" si="3"/>
-        <v>242857.1428571429</v>
+        <f t="shared" ref="V12" si="18">$Z12/21+U12</f>
+        <v>0</v>
       </c>
       <c r="W12">
         <f t="shared" si="1"/>
-        <v>257142.85714285719</v>
+        <v>0</v>
       </c>
       <c r="X12">
         <f t="shared" si="1"/>
-        <v>271428.57142857148</v>
+        <v>0</v>
       </c>
       <c r="Y12">
         <f t="shared" si="1"/>
-        <v>285714.28571428574</v>
-      </c>
-      <c r="Z12" s="20">
-        <f>Sheet1!C15*1000</f>
-        <v>300000</v>
+        <v>0</v>
+      </c>
+      <c r="Z12">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>84</v>
       </c>
       <c r="C13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E13" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="F13" s="20">
         <f>Z13/21</f>
-        <v>0</v>
+        <v>142.85714285714286</v>
       </c>
       <c r="G13">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" ref="G13:P13" si="19">$Z14/21+F13</f>
+        <v>428.57142857142856</v>
       </c>
       <c r="H13">
-        <f t="shared" ref="H13" si="4">$Z13/21+G13</f>
-        <v>0</v>
+        <f t="shared" si="19"/>
+        <v>714.28571428571422</v>
       </c>
       <c r="I13">
-        <f t="shared" ref="I13" si="5">$Z13/21+H13</f>
-        <v>0</v>
+        <f t="shared" si="19"/>
+        <v>1000</v>
       </c>
       <c r="J13">
-        <f t="shared" ref="J13" si="6">$Z13/21+I13</f>
-        <v>0</v>
+        <f t="shared" si="19"/>
+        <v>1285.7142857142858</v>
       </c>
       <c r="K13">
-        <f t="shared" ref="K13" si="7">$Z13/21+J13</f>
-        <v>0</v>
+        <f t="shared" si="19"/>
+        <v>1571.4285714285716</v>
       </c>
       <c r="L13">
-        <f t="shared" ref="L13" si="8">$Z13/21+K13</f>
-        <v>0</v>
+        <f t="shared" si="19"/>
+        <v>1857.1428571428573</v>
       </c>
       <c r="M13">
-        <f t="shared" ref="M13" si="9">$Z13/21+L13</f>
-        <v>0</v>
+        <f t="shared" si="19"/>
+        <v>2142.8571428571431</v>
       </c>
       <c r="N13">
-        <f t="shared" ref="N13" si="10">$Z13/21+M13</f>
-        <v>0</v>
+        <f t="shared" si="19"/>
+        <v>2428.5714285714289</v>
       </c>
       <c r="O13">
-        <f t="shared" ref="O13" si="11">$Z13/21+N13</f>
-        <v>0</v>
+        <f t="shared" si="19"/>
+        <v>2714.2857142857147</v>
       </c>
       <c r="P13">
-        <f t="shared" ref="P13" si="12">$Z13/21+O13</f>
-        <v>0</v>
+        <f t="shared" si="19"/>
+        <v>3000.0000000000005</v>
       </c>
       <c r="Q13">
-        <f t="shared" ref="Q13" si="13">$Z13/21+P13</f>
-        <v>0</v>
+        <f t="shared" ref="Q13:Y13" si="20">$Z14/21+P13</f>
+        <v>3285.7142857142862</v>
       </c>
       <c r="R13">
-        <f t="shared" ref="R13" si="14">$Z13/21+Q13</f>
-        <v>0</v>
+        <f t="shared" si="20"/>
+        <v>3571.428571428572</v>
       </c>
       <c r="S13">
-        <f t="shared" ref="S13" si="15">$Z13/21+R13</f>
-        <v>0</v>
+        <f t="shared" si="20"/>
+        <v>3857.1428571428578</v>
       </c>
       <c r="T13">
-        <f t="shared" ref="T13" si="16">$Z13/21+S13</f>
-        <v>0</v>
+        <f t="shared" si="20"/>
+        <v>4142.8571428571431</v>
       </c>
       <c r="U13">
-        <f t="shared" ref="U13" si="17">$Z13/21+T13</f>
-        <v>0</v>
+        <f t="shared" si="20"/>
+        <v>4428.5714285714284</v>
       </c>
       <c r="V13">
-        <f t="shared" ref="V13" si="18">$Z13/21+U13</f>
-        <v>0</v>
+        <f t="shared" si="20"/>
+        <v>4714.2857142857138</v>
       </c>
       <c r="W13">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="20"/>
+        <v>4999.9999999999991</v>
       </c>
       <c r="X13">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="20"/>
+        <v>5285.7142857142844</v>
       </c>
       <c r="Y13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Z13">
-        <v>0</v>
+        <f t="shared" si="20"/>
+        <v>5571.4285714285697</v>
+      </c>
+      <c r="Z13" s="20">
+        <f>Sheet1!C16*1000</f>
+        <v>3000</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C14" t="s">
         <v>7</v>
@@ -3463,200 +3427,200 @@
         <v>12</v>
       </c>
       <c r="E14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F14" s="20">
         <f>Z14/21</f>
-        <v>142.85714285714286</v>
+        <v>285.71428571428572</v>
       </c>
       <c r="G14">
-        <f t="shared" ref="G14:P14" si="19">$Z15/21+F14</f>
-        <v>428.57142857142856</v>
+        <f>$Z15/21+F14</f>
+        <v>285.71428571428572</v>
       </c>
       <c r="H14">
-        <f t="shared" si="19"/>
-        <v>714.28571428571422</v>
+        <f t="shared" ref="H14:Y14" si="21">$Z15/21+G14</f>
+        <v>285.71428571428572</v>
       </c>
       <c r="I14">
-        <f t="shared" si="19"/>
-        <v>1000</v>
+        <f t="shared" si="21"/>
+        <v>285.71428571428572</v>
       </c>
       <c r="J14">
-        <f t="shared" si="19"/>
-        <v>1285.7142857142858</v>
+        <f t="shared" si="21"/>
+        <v>285.71428571428572</v>
       </c>
       <c r="K14">
-        <f t="shared" si="19"/>
-        <v>1571.4285714285716</v>
+        <f t="shared" si="21"/>
+        <v>285.71428571428572</v>
       </c>
       <c r="L14">
-        <f t="shared" si="19"/>
-        <v>1857.1428571428573</v>
+        <f t="shared" si="21"/>
+        <v>285.71428571428572</v>
       </c>
       <c r="M14">
-        <f t="shared" si="19"/>
-        <v>2142.8571428571431</v>
+        <f t="shared" si="21"/>
+        <v>285.71428571428572</v>
       </c>
       <c r="N14">
-        <f t="shared" si="19"/>
-        <v>2428.5714285714289</v>
+        <f t="shared" si="21"/>
+        <v>285.71428571428572</v>
       </c>
       <c r="O14">
-        <f t="shared" si="19"/>
-        <v>2714.2857142857147</v>
+        <f t="shared" si="21"/>
+        <v>285.71428571428572</v>
       </c>
       <c r="P14">
-        <f t="shared" si="19"/>
-        <v>3000.0000000000005</v>
+        <f t="shared" si="21"/>
+        <v>285.71428571428572</v>
       </c>
       <c r="Q14">
-        <f t="shared" ref="Q14:Y14" si="20">$Z15/21+P14</f>
-        <v>3285.7142857142862</v>
+        <f t="shared" si="21"/>
+        <v>285.71428571428572</v>
       </c>
       <c r="R14">
-        <f t="shared" si="20"/>
-        <v>3571.428571428572</v>
+        <f t="shared" si="21"/>
+        <v>285.71428571428572</v>
       </c>
       <c r="S14">
-        <f t="shared" si="20"/>
-        <v>3857.1428571428578</v>
+        <f t="shared" si="21"/>
+        <v>285.71428571428572</v>
       </c>
       <c r="T14">
-        <f t="shared" si="20"/>
-        <v>4142.8571428571431</v>
+        <f t="shared" si="21"/>
+        <v>285.71428571428572</v>
       </c>
       <c r="U14">
-        <f t="shared" si="20"/>
-        <v>4428.5714285714284</v>
+        <f t="shared" si="21"/>
+        <v>285.71428571428572</v>
       </c>
       <c r="V14">
-        <f t="shared" si="20"/>
-        <v>4714.2857142857138</v>
+        <f t="shared" si="21"/>
+        <v>285.71428571428572</v>
       </c>
       <c r="W14">
-        <f t="shared" si="20"/>
-        <v>4999.9999999999991</v>
+        <f t="shared" si="21"/>
+        <v>285.71428571428572</v>
       </c>
       <c r="X14">
-        <f t="shared" si="20"/>
-        <v>5285.7142857142844</v>
+        <f t="shared" si="21"/>
+        <v>285.71428571428572</v>
       </c>
       <c r="Y14">
-        <f t="shared" si="20"/>
-        <v>5571.4285714285697</v>
+        <f t="shared" si="21"/>
+        <v>285.71428571428572</v>
       </c>
       <c r="Z14" s="20">
-        <f>Sheet1!C16*1000</f>
-        <v>3000</v>
+        <f>Sheet1!C17*1000</f>
+        <v>6000</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C15" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D15" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E15" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F15" s="20">
-        <f>Z15/21</f>
-        <v>285.71428571428572</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="G15">
-        <f>$Z16/21+F15</f>
-        <v>285.71428571428572</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="H15">
-        <f t="shared" ref="H15:Y15" si="21">$Z16/21+G15</f>
-        <v>285.71428571428572</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="I15">
-        <f t="shared" si="21"/>
-        <v>285.71428571428572</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="J15">
-        <f t="shared" si="21"/>
-        <v>285.71428571428572</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="K15">
-        <f t="shared" si="21"/>
-        <v>285.71428571428572</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="L15">
-        <f t="shared" si="21"/>
-        <v>285.71428571428572</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="M15">
-        <f t="shared" si="21"/>
-        <v>285.71428571428572</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="N15">
-        <f t="shared" si="21"/>
-        <v>285.71428571428572</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="O15">
-        <f t="shared" si="21"/>
-        <v>285.71428571428572</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="P15">
-        <f t="shared" si="21"/>
-        <v>285.71428571428572</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="21"/>
-        <v>285.71428571428572</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="R15">
-        <f t="shared" si="21"/>
-        <v>285.71428571428572</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="S15">
-        <f t="shared" si="21"/>
-        <v>285.71428571428572</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="T15">
-        <f t="shared" si="21"/>
-        <v>285.71428571428572</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="U15">
-        <f t="shared" si="21"/>
-        <v>285.71428571428572</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="V15">
-        <f t="shared" si="21"/>
-        <v>285.71428571428572</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="W15">
-        <f t="shared" si="21"/>
-        <v>285.71428571428572</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="X15">
-        <f t="shared" si="21"/>
-        <v>285.71428571428572</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="Y15">
-        <f t="shared" si="21"/>
-        <v>285.71428571428572</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="Z15" s="20">
-        <f>Sheet1!C17*1000</f>
-        <v>6000</v>
+        <f>Sheet1!C19*1000</f>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C16" t="s">
         <v>15</v>
@@ -3665,7 +3629,7 @@
         <v>16</v>
       </c>
       <c r="E16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F16" s="20">
         <f t="shared" si="2"/>
@@ -3748,16 +3712,15 @@
         <v>0</v>
       </c>
       <c r="Z16" s="20">
-        <f>Sheet1!C19*1000</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>95</v>
       </c>
       <c r="B17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C17" t="s">
         <v>15</v>
@@ -3766,189 +3729,89 @@
         <v>16</v>
       </c>
       <c r="E17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F17" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.23809523809523808</v>
       </c>
       <c r="G17">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.47619047619047616</v>
       </c>
       <c r="H17">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.71428571428571419</v>
       </c>
       <c r="I17">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.95238095238095233</v>
       </c>
       <c r="J17">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1.1904761904761905</v>
       </c>
       <c r="K17">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1.4285714285714286</v>
       </c>
       <c r="L17">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="M17">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1.9047619047619049</v>
       </c>
       <c r="N17">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2.1428571428571428</v>
       </c>
       <c r="O17">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2.3809523809523809</v>
       </c>
       <c r="P17">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2.6190476190476191</v>
       </c>
       <c r="Q17">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2.8571428571428572</v>
       </c>
       <c r="R17">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3.0952380952380953</v>
       </c>
       <c r="S17">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3.3333333333333335</v>
       </c>
       <c r="T17">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3.5714285714285716</v>
       </c>
       <c r="U17">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3.8095238095238098</v>
       </c>
       <c r="V17">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" ref="V17:Y17" si="22">$Z17/21+U17</f>
+        <v>4.0476190476190474</v>
       </c>
       <c r="W17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Y17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Z17" s="20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>96</v>
-      </c>
-      <c r="B18" t="s">
-        <v>89</v>
-      </c>
-      <c r="C18" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" t="s">
-        <v>88</v>
-      </c>
-      <c r="F18" s="20">
-        <f t="shared" si="2"/>
-        <v>0.23809523809523808</v>
-      </c>
-      <c r="G18">
-        <f t="shared" si="3"/>
-        <v>0.47619047619047616</v>
-      </c>
-      <c r="H18">
-        <f t="shared" si="3"/>
-        <v>0.71428571428571419</v>
-      </c>
-      <c r="I18">
-        <f t="shared" si="3"/>
-        <v>0.95238095238095233</v>
-      </c>
-      <c r="J18">
-        <f t="shared" si="3"/>
-        <v>1.1904761904761905</v>
-      </c>
-      <c r="K18">
-        <f t="shared" si="3"/>
-        <v>1.4285714285714286</v>
-      </c>
-      <c r="L18">
-        <f t="shared" si="3"/>
-        <v>1.6666666666666667</v>
-      </c>
-      <c r="M18">
-        <f t="shared" si="3"/>
-        <v>1.9047619047619049</v>
-      </c>
-      <c r="N18">
-        <f t="shared" si="3"/>
-        <v>2.1428571428571428</v>
-      </c>
-      <c r="O18">
-        <f t="shared" si="3"/>
-        <v>2.3809523809523809</v>
-      </c>
-      <c r="P18">
-        <f t="shared" si="3"/>
-        <v>2.6190476190476191</v>
-      </c>
-      <c r="Q18">
-        <f t="shared" si="3"/>
-        <v>2.8571428571428572</v>
-      </c>
-      <c r="R18">
-        <f t="shared" si="3"/>
-        <v>3.0952380952380953</v>
-      </c>
-      <c r="S18">
-        <f t="shared" si="3"/>
-        <v>3.3333333333333335</v>
-      </c>
-      <c r="T18">
-        <f t="shared" si="3"/>
-        <v>3.5714285714285716</v>
-      </c>
-      <c r="U18">
-        <f t="shared" si="3"/>
-        <v>3.8095238095238098</v>
-      </c>
-      <c r="V18">
-        <f t="shared" ref="V18:Y18" si="22">$Z18/21+U18</f>
-        <v>4.0476190476190474</v>
-      </c>
-      <c r="W18">
         <f t="shared" si="22"/>
         <v>4.2857142857142856</v>
       </c>
-      <c r="X18">
+      <c r="X17">
         <f t="shared" si="22"/>
         <v>4.5238095238095237</v>
       </c>
-      <c r="Y18">
+      <c r="Y17">
         <f t="shared" si="22"/>
         <v>4.7619047619047619</v>
       </c>
-      <c r="Z18" s="20">
+      <c r="Z17" s="20">
         <f>Sheet1!C20+Sheet1!C21</f>
         <v>5</v>
       </c>
@@ -4005,7 +3868,7 @@
         <v>64</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed EB's Expected Portfolio
</commit_message>
<xml_diff>
--- a/data/SJV Portfolio Tool Spreadsheet - EBetancourt-TheExpectedPortfolio EDITED.xlsx
+++ b/data/SJV Portfolio Tool Spreadsheet - EBetancourt-TheExpectedPortfolio EDITED.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nidhi/Library/CloudStorage/OneDrive-RANDCorporation/CATF/SJV-/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DDD17DC-20A6-F54F-99F1-2F011817E9AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD245A7-F57E-C54D-B6BA-0613E83CDB06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20800" activeTab="1" xr2:uid="{3EB5D1B8-C67A-D54A-8FBA-1478F31DBAA7}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20800" activeTab="2" xr2:uid="{3EB5D1B8-C67A-D54A-8FBA-1478F31DBAA7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1478,7 +1478,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FAF5C93-78A2-4745-8CA2-3B35004E83AD}">
   <dimension ref="A1:W8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
@@ -2107,8 +2107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AB86C67-1FB8-CB44-BDCD-F09BD6DE6122}">
   <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3330,80 +3330,80 @@
         <v>142.85714285714286</v>
       </c>
       <c r="G13">
-        <f t="shared" ref="G13:P13" si="19">$Z14/21+F13</f>
-        <v>428.57142857142856</v>
+        <f>$Z13/21+F13</f>
+        <v>285.71428571428572</v>
       </c>
       <c r="H13">
-        <f t="shared" si="19"/>
-        <v>714.28571428571422</v>
+        <f t="shared" ref="G13:P13" si="19">$Z14/21+G13</f>
+        <v>571.42857142857144</v>
       </c>
       <c r="I13">
         <f t="shared" si="19"/>
-        <v>1000</v>
+        <v>857.14285714285711</v>
       </c>
       <c r="J13">
         <f t="shared" si="19"/>
-        <v>1285.7142857142858</v>
+        <v>1142.8571428571429</v>
       </c>
       <c r="K13">
         <f t="shared" si="19"/>
-        <v>1571.4285714285716</v>
+        <v>1428.5714285714287</v>
       </c>
       <c r="L13">
         <f t="shared" si="19"/>
-        <v>1857.1428571428573</v>
+        <v>1714.2857142857144</v>
       </c>
       <c r="M13">
         <f t="shared" si="19"/>
-        <v>2142.8571428571431</v>
+        <v>2000.0000000000002</v>
       </c>
       <c r="N13">
         <f t="shared" si="19"/>
-        <v>2428.5714285714289</v>
+        <v>2285.7142857142858</v>
       </c>
       <c r="O13">
         <f t="shared" si="19"/>
-        <v>2714.2857142857147</v>
+        <v>2571.4285714285716</v>
       </c>
       <c r="P13">
         <f t="shared" si="19"/>
-        <v>3000.0000000000005</v>
+        <v>2857.1428571428573</v>
       </c>
       <c r="Q13">
         <f t="shared" ref="Q13:Y13" si="20">$Z14/21+P13</f>
-        <v>3285.7142857142862</v>
+        <v>3142.8571428571431</v>
       </c>
       <c r="R13">
         <f t="shared" si="20"/>
-        <v>3571.428571428572</v>
+        <v>3428.5714285714289</v>
       </c>
       <c r="S13">
         <f t="shared" si="20"/>
-        <v>3857.1428571428578</v>
+        <v>3714.2857142857147</v>
       </c>
       <c r="T13">
         <f t="shared" si="20"/>
-        <v>4142.8571428571431</v>
+        <v>4000.0000000000005</v>
       </c>
       <c r="U13">
         <f t="shared" si="20"/>
-        <v>4428.5714285714284</v>
+        <v>4285.7142857142862</v>
       </c>
       <c r="V13">
         <f t="shared" si="20"/>
-        <v>4714.2857142857138</v>
+        <v>4571.4285714285716</v>
       </c>
       <c r="W13">
         <f t="shared" si="20"/>
-        <v>4999.9999999999991</v>
+        <v>4857.1428571428569</v>
       </c>
       <c r="X13">
         <f t="shared" si="20"/>
-        <v>5285.7142857142844</v>
+        <v>5142.8571428571422</v>
       </c>
       <c r="Y13">
         <f t="shared" si="20"/>
-        <v>5571.4285714285697</v>
+        <v>5428.5714285714275</v>
       </c>
       <c r="Z13" s="20">
         <f>Sheet1!C16*1000</f>
@@ -3431,80 +3431,80 @@
         <v>285.71428571428572</v>
       </c>
       <c r="G14">
-        <f>$Z15/21+F14</f>
-        <v>285.71428571428572</v>
+        <f>$Z14/21+F14</f>
+        <v>571.42857142857144</v>
       </c>
       <c r="H14">
         <f t="shared" ref="H14:Y14" si="21">$Z15/21+G14</f>
-        <v>285.71428571428572</v>
+        <v>571.42857142857144</v>
       </c>
       <c r="I14">
         <f t="shared" si="21"/>
-        <v>285.71428571428572</v>
+        <v>571.42857142857144</v>
       </c>
       <c r="J14">
         <f t="shared" si="21"/>
-        <v>285.71428571428572</v>
+        <v>571.42857142857144</v>
       </c>
       <c r="K14">
         <f t="shared" si="21"/>
-        <v>285.71428571428572</v>
+        <v>571.42857142857144</v>
       </c>
       <c r="L14">
         <f t="shared" si="21"/>
-        <v>285.71428571428572</v>
+        <v>571.42857142857144</v>
       </c>
       <c r="M14">
         <f t="shared" si="21"/>
-        <v>285.71428571428572</v>
+        <v>571.42857142857144</v>
       </c>
       <c r="N14">
         <f t="shared" si="21"/>
-        <v>285.71428571428572</v>
+        <v>571.42857142857144</v>
       </c>
       <c r="O14">
         <f t="shared" si="21"/>
-        <v>285.71428571428572</v>
+        <v>571.42857142857144</v>
       </c>
       <c r="P14">
         <f t="shared" si="21"/>
-        <v>285.71428571428572</v>
+        <v>571.42857142857144</v>
       </c>
       <c r="Q14">
         <f t="shared" si="21"/>
-        <v>285.71428571428572</v>
+        <v>571.42857142857144</v>
       </c>
       <c r="R14">
         <f t="shared" si="21"/>
-        <v>285.71428571428572</v>
+        <v>571.42857142857144</v>
       </c>
       <c r="S14">
         <f t="shared" si="21"/>
-        <v>285.71428571428572</v>
+        <v>571.42857142857144</v>
       </c>
       <c r="T14">
         <f t="shared" si="21"/>
-        <v>285.71428571428572</v>
+        <v>571.42857142857144</v>
       </c>
       <c r="U14">
         <f t="shared" si="21"/>
-        <v>285.71428571428572</v>
+        <v>571.42857142857144</v>
       </c>
       <c r="V14">
         <f t="shared" si="21"/>
-        <v>285.71428571428572</v>
+        <v>571.42857142857144</v>
       </c>
       <c r="W14">
         <f t="shared" si="21"/>
-        <v>285.71428571428572</v>
+        <v>571.42857142857144</v>
       </c>
       <c r="X14">
         <f t="shared" si="21"/>
-        <v>285.71428571428572</v>
+        <v>571.42857142857144</v>
       </c>
       <c r="Y14">
         <f t="shared" si="21"/>
-        <v>285.71428571428572</v>
+        <v>571.42857142857144</v>
       </c>
       <c r="Z14" s="20">
         <f>Sheet1!C17*1000</f>

</xml_diff>

<commit_message>
Anotehr fix of EB portfolio
</commit_message>
<xml_diff>
--- a/data/SJV Portfolio Tool Spreadsheet - EBetancourt-TheExpectedPortfolio EDITED.xlsx
+++ b/data/SJV Portfolio Tool Spreadsheet - EBetancourt-TheExpectedPortfolio EDITED.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nidhi/Library/CloudStorage/OneDrive-RANDCorporation/CATF/SJV-/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD245A7-F57E-C54D-B6BA-0613E83CDB06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2071FA0E-2D67-AF4D-B36E-3F610A3B686E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20800" activeTab="2" xr2:uid="{3EB5D1B8-C67A-D54A-8FBA-1478F31DBAA7}"/>
   </bookViews>
@@ -2108,7 +2108,7 @@
   <dimension ref="A1:Z17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="Y1" sqref="Y1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3238,59 +3238,59 @@
         <v>0</v>
       </c>
       <c r="I12">
-        <f t="shared" ref="I12" si="5">$Z12/21+H12</f>
+        <f t="shared" ref="I12:I13" si="5">$Z12/21+H12</f>
         <v>0</v>
       </c>
       <c r="J12">
-        <f t="shared" ref="J12" si="6">$Z12/21+I12</f>
+        <f t="shared" ref="J12:J13" si="6">$Z12/21+I12</f>
         <v>0</v>
       </c>
       <c r="K12">
-        <f t="shared" ref="K12" si="7">$Z12/21+J12</f>
+        <f t="shared" ref="K12:K13" si="7">$Z12/21+J12</f>
         <v>0</v>
       </c>
       <c r="L12">
-        <f t="shared" ref="L12" si="8">$Z12/21+K12</f>
+        <f t="shared" ref="L12:L13" si="8">$Z12/21+K12</f>
         <v>0</v>
       </c>
       <c r="M12">
-        <f t="shared" ref="M12" si="9">$Z12/21+L12</f>
+        <f t="shared" ref="M12:M13" si="9">$Z12/21+L12</f>
         <v>0</v>
       </c>
       <c r="N12">
-        <f t="shared" ref="N12" si="10">$Z12/21+M12</f>
+        <f t="shared" ref="N12:N13" si="10">$Z12/21+M12</f>
         <v>0</v>
       </c>
       <c r="O12">
-        <f t="shared" ref="O12" si="11">$Z12/21+N12</f>
+        <f t="shared" ref="O12:O13" si="11">$Z12/21+N12</f>
         <v>0</v>
       </c>
       <c r="P12">
-        <f t="shared" ref="P12" si="12">$Z12/21+O12</f>
+        <f t="shared" ref="P12:P13" si="12">$Z12/21+O12</f>
         <v>0</v>
       </c>
       <c r="Q12">
-        <f t="shared" ref="Q12" si="13">$Z12/21+P12</f>
+        <f t="shared" ref="Q12:Q13" si="13">$Z12/21+P12</f>
         <v>0</v>
       </c>
       <c r="R12">
-        <f t="shared" ref="R12" si="14">$Z12/21+Q12</f>
+        <f t="shared" ref="R12:R13" si="14">$Z12/21+Q12</f>
         <v>0</v>
       </c>
       <c r="S12">
-        <f t="shared" ref="S12" si="15">$Z12/21+R12</f>
+        <f t="shared" ref="S12:S13" si="15">$Z12/21+R12</f>
         <v>0</v>
       </c>
       <c r="T12">
-        <f t="shared" ref="T12" si="16">$Z12/21+S12</f>
+        <f t="shared" ref="T12:T13" si="16">$Z12/21+S12</f>
         <v>0</v>
       </c>
       <c r="U12">
-        <f t="shared" ref="U12" si="17">$Z12/21+T12</f>
+        <f t="shared" ref="U12:U13" si="17">$Z12/21+T12</f>
         <v>0</v>
       </c>
       <c r="V12">
-        <f t="shared" ref="V12" si="18">$Z12/21+U12</f>
+        <f t="shared" ref="V12:V13" si="18">$Z12/21+U12</f>
         <v>0</v>
       </c>
       <c r="W12">
@@ -3334,76 +3334,76 @@
         <v>285.71428571428572</v>
       </c>
       <c r="H13">
-        <f t="shared" ref="G13:P13" si="19">$Z14/21+G13</f>
+        <f>$Z13/21+G13</f>
+        <v>428.57142857142856</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="5"/>
         <v>571.42857142857144</v>
       </c>
-      <c r="I13">
-        <f t="shared" si="19"/>
-        <v>857.14285714285711</v>
-      </c>
       <c r="J13">
-        <f t="shared" si="19"/>
+        <f t="shared" si="6"/>
+        <v>714.28571428571433</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="7"/>
+        <v>857.14285714285722</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="8"/>
+        <v>1000.0000000000001</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="9"/>
         <v>1142.8571428571429</v>
       </c>
-      <c r="K13">
-        <f t="shared" si="19"/>
+      <c r="N13">
+        <f t="shared" si="10"/>
+        <v>1285.7142857142858</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="11"/>
         <v>1428.5714285714287</v>
       </c>
-      <c r="L13">
-        <f t="shared" si="19"/>
+      <c r="P13">
+        <f t="shared" si="12"/>
+        <v>1571.4285714285716</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="13"/>
         <v>1714.2857142857144</v>
       </c>
-      <c r="M13">
-        <f t="shared" si="19"/>
+      <c r="R13">
+        <f t="shared" si="14"/>
+        <v>1857.1428571428573</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="15"/>
         <v>2000.0000000000002</v>
       </c>
-      <c r="N13">
-        <f t="shared" si="19"/>
+      <c r="T13">
+        <f t="shared" si="16"/>
+        <v>2142.8571428571431</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="17"/>
         <v>2285.7142857142858</v>
       </c>
-      <c r="O13">
-        <f t="shared" si="19"/>
-        <v>2571.4285714285716</v>
-      </c>
-      <c r="P13">
-        <f t="shared" si="19"/>
-        <v>2857.1428571428573</v>
-      </c>
-      <c r="Q13">
-        <f t="shared" ref="Q13:Y13" si="20">$Z14/21+P13</f>
-        <v>3142.8571428571431</v>
-      </c>
-      <c r="R13">
-        <f t="shared" si="20"/>
-        <v>3428.5714285714289</v>
-      </c>
-      <c r="S13">
-        <f t="shared" si="20"/>
-        <v>3714.2857142857147</v>
-      </c>
-      <c r="T13">
-        <f t="shared" si="20"/>
-        <v>4000.0000000000005</v>
-      </c>
-      <c r="U13">
-        <f t="shared" si="20"/>
-        <v>4285.7142857142862</v>
-      </c>
       <c r="V13">
-        <f t="shared" si="20"/>
-        <v>4571.4285714285716</v>
+        <f t="shared" si="18"/>
+        <v>2428.5714285714284</v>
       </c>
       <c r="W13">
-        <f t="shared" si="20"/>
-        <v>4857.1428571428569</v>
+        <f t="shared" si="1"/>
+        <v>2571.4285714285711</v>
       </c>
       <c r="X13">
-        <f t="shared" si="20"/>
-        <v>5142.8571428571422</v>
+        <f t="shared" si="1"/>
+        <v>2714.2857142857138</v>
       </c>
       <c r="Y13">
-        <f t="shared" si="20"/>
-        <v>5428.5714285714275</v>
+        <f t="shared" si="1"/>
+        <v>2857.1428571428564</v>
       </c>
       <c r="Z13" s="20">
         <f>Sheet1!C16*1000</f>
@@ -3435,76 +3435,76 @@
         <v>571.42857142857144</v>
       </c>
       <c r="H14">
-        <f t="shared" ref="H14:Y14" si="21">$Z15/21+G14</f>
-        <v>571.42857142857144</v>
+        <f t="shared" ref="H14:Y14" si="19">$Z14/21+G14</f>
+        <v>857.14285714285711</v>
       </c>
       <c r="I14">
-        <f t="shared" si="21"/>
-        <v>571.42857142857144</v>
+        <f t="shared" si="19"/>
+        <v>1142.8571428571429</v>
       </c>
       <c r="J14">
-        <f t="shared" si="21"/>
-        <v>571.42857142857144</v>
+        <f t="shared" si="19"/>
+        <v>1428.5714285714287</v>
       </c>
       <c r="K14">
-        <f t="shared" si="21"/>
-        <v>571.42857142857144</v>
+        <f t="shared" si="19"/>
+        <v>1714.2857142857144</v>
       </c>
       <c r="L14">
-        <f t="shared" si="21"/>
-        <v>571.42857142857144</v>
+        <f t="shared" si="19"/>
+        <v>2000.0000000000002</v>
       </c>
       <c r="M14">
-        <f t="shared" si="21"/>
-        <v>571.42857142857144</v>
+        <f t="shared" si="19"/>
+        <v>2285.7142857142858</v>
       </c>
       <c r="N14">
-        <f t="shared" si="21"/>
-        <v>571.42857142857144</v>
+        <f t="shared" si="19"/>
+        <v>2571.4285714285716</v>
       </c>
       <c r="O14">
-        <f t="shared" si="21"/>
-        <v>571.42857142857144</v>
+        <f t="shared" si="19"/>
+        <v>2857.1428571428573</v>
       </c>
       <c r="P14">
-        <f t="shared" si="21"/>
-        <v>571.42857142857144</v>
+        <f t="shared" si="19"/>
+        <v>3142.8571428571431</v>
       </c>
       <c r="Q14">
-        <f t="shared" si="21"/>
-        <v>571.42857142857144</v>
+        <f t="shared" si="19"/>
+        <v>3428.5714285714289</v>
       </c>
       <c r="R14">
-        <f t="shared" si="21"/>
-        <v>571.42857142857144</v>
+        <f t="shared" si="19"/>
+        <v>3714.2857142857147</v>
       </c>
       <c r="S14">
-        <f t="shared" si="21"/>
-        <v>571.42857142857144</v>
+        <f t="shared" si="19"/>
+        <v>4000.0000000000005</v>
       </c>
       <c r="T14">
-        <f t="shared" si="21"/>
-        <v>571.42857142857144</v>
+        <f t="shared" si="19"/>
+        <v>4285.7142857142862</v>
       </c>
       <c r="U14">
-        <f t="shared" si="21"/>
-        <v>571.42857142857144</v>
+        <f t="shared" si="19"/>
+        <v>4571.4285714285716</v>
       </c>
       <c r="V14">
-        <f t="shared" si="21"/>
-        <v>571.42857142857144</v>
+        <f t="shared" si="19"/>
+        <v>4857.1428571428569</v>
       </c>
       <c r="W14">
-        <f t="shared" si="21"/>
-        <v>571.42857142857144</v>
+        <f t="shared" si="19"/>
+        <v>5142.8571428571422</v>
       </c>
       <c r="X14">
-        <f t="shared" si="21"/>
-        <v>571.42857142857144</v>
+        <f t="shared" si="19"/>
+        <v>5428.5714285714275</v>
       </c>
       <c r="Y14">
-        <f t="shared" si="21"/>
-        <v>571.42857142857144</v>
+        <f t="shared" si="19"/>
+        <v>5714.2857142857129</v>
       </c>
       <c r="Z14" s="20">
         <f>Sheet1!C17*1000</f>
@@ -3793,19 +3793,19 @@
         <v>3.8095238095238098</v>
       </c>
       <c r="V17">
-        <f t="shared" ref="V17:Y17" si="22">$Z17/21+U17</f>
+        <f t="shared" ref="V17:Y17" si="20">$Z17/21+U17</f>
         <v>4.0476190476190474</v>
       </c>
       <c r="W17">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>4.2857142857142856</v>
       </c>
       <c r="X17">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>4.5238095238095237</v>
       </c>
       <c r="Y17">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>4.7619047619047619</v>
       </c>
       <c r="Z17" s="20">

</xml_diff>